<commit_message>
first charts and overall check on footprint of capacity
</commit_message>
<xml_diff>
--- a/Shocks/Shock_files/Constant_2011_Average.xlsx
+++ b/Shocks/Shock_files/Constant_2011_Average.xlsx
@@ -11035,7 +11035,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11093,36 +11093,36 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Production of photovoltaic plants</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>EU27+UK</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Commodity</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Photovoltaic plants</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>EU27+UK</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Production of electricity by solar photovoltaic</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>Update</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.2384371777875976</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -11133,36 +11133,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Production of onshore wind plants</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>EU27+UK</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Commodity</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Onshore wind plants</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>EU27+UK</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Production of electricity by wind</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Update</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.0540339865508731</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -11173,35 +11173,155 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Production of offshore wind plants</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>EU27+UK</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Commodity</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Offshore wind plants</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>EU27+UK</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Photovoltaic plants</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>EU27+UK</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>Activity</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Production of electricity by solar photovoltaic</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0.2384371777875976</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>EU27+UK</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Onshore wind plants</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>EU27+UK</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Production of electricity by wind</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Update</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="H6" t="n">
+        <v>0.0540339865508731</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>EU27+UK</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Offshore wind plants</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EU27+UK</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Production of electricity by wind</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Update</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
         <v>0.1049820613176778</v>
       </c>
     </row>

</xml_diff>

<commit_message>
price logic changed based on Exiobase Energy Carrier Supply Total (scenario=constant for now)
</commit_message>
<xml_diff>
--- a/Shocks/Shock_files/Constant_2011_Average.xlsx
+++ b/Shocks/Shock_files/Constant_2011_Average.xlsx
@@ -10636,7 +10636,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.2321248222124024</v>
+        <v>0.05601883435997856</v>
       </c>
     </row>
     <row r="3">
@@ -10666,7 +10666,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.2938729521314491</v>
+        <v>0.1764261745184988</v>
       </c>
     </row>
   </sheetData>
@@ -11242,7 +11242,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.2384371777875976</v>
+        <v>0.4145431656400214</v>
       </c>
     </row>
     <row r="6">
@@ -11282,7 +11282,7 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.0540339865508731</v>
+        <v>0.09394264789068643</v>
       </c>
     </row>
     <row r="7">
@@ -11322,7 +11322,7 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>0.1049820613176778</v>
+        <v>0.1825201775908148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>